<commit_message>
included 500 print area
</commit_message>
<xml_diff>
--- a/FirmWareSettings.xlsx
+++ b/FirmWareSettings.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivi\OneDrive\Documents\GitHub\HevORT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0174A839-2023-4943-BA64-6E420B2FF5EF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D68B6714-F2ED-4709-AC29-15A62BF7BF8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{509C0CBF-6515-4E03-BB96-B231BA0137C3}"/>
   </bookViews>
@@ -1149,6 +1149,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1211,23 +1228,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -6673,10 +6673,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EBDBAD23-474B-4AC5-A011-4D1EC1466E50}" name="Table2" displayName="Table2" ref="H2:J16" totalsRowShown="0">
-  <autoFilter ref="H2:J16" xr:uid="{8764FB30-DFE5-42AF-8A36-D229AA709EFC}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="H3:J16">
-    <sortCondition ref="H2:H16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EBDBAD23-474B-4AC5-A011-4D1EC1466E50}" name="Table2" displayName="Table2" ref="H2:J17" totalsRowShown="0">
+  <autoFilter ref="H2:J17" xr:uid="{8764FB30-DFE5-42AF-8A36-D229AA709EFC}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="H3:J17">
+    <sortCondition ref="H2:H17"/>
   </sortState>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{1C84F27E-F9F2-4C03-8F9F-A726A1A6B86A}" name="PrintArea"/>
@@ -6993,8 +6993,8 @@
   </sheetPr>
   <dimension ref="A1:U50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7026,15 +7026,15 @@
         <v>1</v>
       </c>
       <c r="B2" s="8">
-        <v>315</v>
+        <v>500</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="38" t="s">
+      <c r="I2" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="39"/>
+      <c r="J2" s="50"/>
     </row>
     <row r="3" spans="1:10" ht="26" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
@@ -7046,14 +7046,14 @@
       <c r="C3" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="40"/>
-      <c r="J3" s="41"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="52"/>
     </row>
     <row r="4" spans="1:10" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="I4" s="44" t="s">
+      <c r="I4" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="45"/>
+      <c r="J4" s="56"/>
     </row>
     <row r="5" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A5" s="10" t="s">
@@ -7081,11 +7081,11 @@
       </c>
       <c r="I6" s="15">
         <f>B41+(K50/2)</f>
-        <v>138.02100000000002</v>
+        <v>230.52100000000002</v>
       </c>
       <c r="J6" s="15">
         <f>C41+S27</f>
-        <v>307.49299999999999</v>
+        <v>492.49300000000005</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
@@ -7105,7 +7105,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="26" x14ac:dyDescent="0.6">
-      <c r="A11" s="60" t="s">
+      <c r="A11" s="39" t="s">
         <v>61</v>
       </c>
       <c r="B11" s="21"/>
@@ -7133,9 +7133,9 @@
       <c r="F13" s="25"/>
     </row>
     <row r="14" spans="1:10" ht="28.5" x14ac:dyDescent="0.65">
-      <c r="A14" s="61" t="str">
+      <c r="A14" s="40" t="str">
         <f xml:space="preserve"> "M671 " &amp; "X" &amp; B41 &amp; ":" &amp; I6 &amp; ":" &amp; T41 &amp; " Y" &amp; C41 &amp; ":" &amp; J6 &amp; ":" &amp; U41 &amp; " S50"</f>
-        <v>M671 X-38.188:138.021:314.23 Y-20.717:307.493:-20.717 S50</v>
+        <v>M671 X-38.188:230.521:499.23 Y-20.717:492.493:-20.717 S50</v>
       </c>
       <c r="B14" s="30"/>
       <c r="C14" s="30"/>
@@ -7162,7 +7162,7 @@
       <c r="F16" s="25"/>
     </row>
     <row r="17" spans="1:19" ht="21.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="62" t="str">
+      <c r="A17" s="41" t="str">
         <f>"G31 P500 X"&amp;VLOOKUP(B3,Table1[],4,0) &amp; " Y"&amp; VLOOKUP(B3,Table1[],5,0) &amp; " Z[measured via Paper technique]"</f>
         <v>G31 P500 X22.775 Y5.21 Z[measured via Paper technique]</v>
       </c>
@@ -7174,43 +7174,43 @@
     </row>
     <row r="19" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="20" spans="1:19" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="67" t="s">
+      <c r="A20" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="B20" s="63"/>
+      <c r="B20" s="42"/>
     </row>
     <row r="21" spans="1:19" ht="21" x14ac:dyDescent="0.5">
-      <c r="A21" s="64" t="s">
+      <c r="A21" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="B21" s="65"/>
+      <c r="B21" s="44"/>
     </row>
     <row r="22" spans="1:19" ht="21" x14ac:dyDescent="0.5">
-      <c r="A22" s="64" t="s">
+      <c r="A22" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="B22" s="65"/>
+      <c r="B22" s="44"/>
     </row>
     <row r="23" spans="1:19" ht="21" x14ac:dyDescent="0.5">
-      <c r="A23" s="68" t="str">
+      <c r="A23" s="47" t="str">
         <f>B41&amp;","&amp;C41</f>
         <v>-38.188,-20.717</v>
       </c>
-      <c r="B23" s="65"/>
+      <c r="B23" s="44"/>
     </row>
     <row r="24" spans="1:19" ht="21" x14ac:dyDescent="0.5">
-      <c r="A24" s="68" t="str">
+      <c r="A24" s="47" t="str">
         <f>I6&amp;","&amp;J6</f>
-        <v>138.021,307.493</v>
-      </c>
-      <c r="B24" s="65"/>
+        <v>230.521,492.493</v>
+      </c>
+      <c r="B24" s="44"/>
     </row>
     <row r="25" spans="1:19" ht="21.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="69" t="str">
+      <c r="A25" s="48" t="str">
         <f>T41&amp;","&amp;U41</f>
-        <v>314.23,-20.717</v>
-      </c>
-      <c r="B25" s="66"/>
+        <v>499.23,-20.717</v>
+      </c>
+      <c r="B25" s="45"/>
     </row>
     <row r="27" spans="1:19" ht="28.5" x14ac:dyDescent="0.65">
       <c r="A27" s="5"/>
@@ -7219,11 +7219,11 @@
       </c>
       <c r="S27" s="16">
         <f>VLOOKUP(B2,DATA!H:J,3,0)</f>
-        <v>328.21</v>
+        <v>513.21</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A28" s="59"/>
+      <c r="A28" s="38"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A29" s="5"/>
@@ -7234,42 +7234,42 @@
       </c>
     </row>
     <row r="35" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B35" s="38" t="s">
+      <c r="B35" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="C35" s="39"/>
-      <c r="T35" s="38" t="s">
+      <c r="C35" s="50"/>
+      <c r="T35" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="U35" s="39"/>
+      <c r="U35" s="50"/>
     </row>
     <row r="36" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B36" s="40"/>
-      <c r="C36" s="41"/>
-      <c r="T36" s="40"/>
-      <c r="U36" s="41"/>
+      <c r="B36" s="51"/>
+      <c r="C36" s="52"/>
+      <c r="T36" s="51"/>
+      <c r="U36" s="52"/>
     </row>
     <row r="37" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B37" s="40"/>
-      <c r="C37" s="41"/>
-      <c r="T37" s="40"/>
-      <c r="U37" s="41"/>
+      <c r="B37" s="51"/>
+      <c r="C37" s="52"/>
+      <c r="T37" s="51"/>
+      <c r="U37" s="52"/>
     </row>
     <row r="38" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B38" s="46"/>
-      <c r="C38" s="47"/>
-      <c r="T38" s="46"/>
-      <c r="U38" s="47"/>
+      <c r="B38" s="57"/>
+      <c r="C38" s="58"/>
+      <c r="T38" s="57"/>
+      <c r="U38" s="58"/>
     </row>
     <row r="39" spans="2:21" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="B39" s="42" t="s">
+      <c r="B39" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="C39" s="43"/>
-      <c r="T39" s="42" t="s">
+      <c r="C39" s="54"/>
+      <c r="T39" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="U39" s="43"/>
+      <c r="U39" s="54"/>
     </row>
     <row r="40" spans="2:21" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B40" s="17" t="s">
@@ -7296,7 +7296,7 @@
       </c>
       <c r="T41" s="19">
         <f>B41+(K50)</f>
-        <v>314.23</v>
+        <v>499.23</v>
       </c>
       <c r="U41" s="20">
         <f>C41</f>
@@ -7306,7 +7306,7 @@
     <row r="50" spans="11:11" ht="28.5" x14ac:dyDescent="0.65">
       <c r="K50" s="16">
         <f>VLOOKUP(B2,DATA!H:J,2,0)</f>
-        <v>352.41800000000001</v>
+        <v>537.41800000000001</v>
       </c>
     </row>
   </sheetData>
@@ -7332,7 +7332,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4D9FCBA9-6355-4BD1-B57E-30257C3D0E30}">
           <x14:formula1>
-            <xm:f>DATA!$H$3:$H$16</xm:f>
+            <xm:f>DATA!$H$3:$H$17</xm:f>
           </x14:formula1>
           <xm:sqref>B2</xm:sqref>
         </x14:dataValidation>
@@ -7356,46 +7356,46 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:30" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="63" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="Z3" s="52" t="s">
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="Z3" s="63" t="s">
         <v>39</v>
       </c>
-      <c r="AA3" s="52"/>
-      <c r="AB3" s="52"/>
-      <c r="AC3" s="52"/>
-      <c r="AD3" s="52"/>
+      <c r="AA3" s="63"/>
+      <c r="AB3" s="63"/>
+      <c r="AC3" s="63"/>
+      <c r="AD3" s="63"/>
     </row>
     <row r="4" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
-      <c r="Z4" s="52"/>
-      <c r="AA4" s="52"/>
-      <c r="AB4" s="52"/>
-      <c r="AC4" s="52"/>
-      <c r="AD4" s="52"/>
+      <c r="B4" s="63"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="Z4" s="63"/>
+      <c r="AA4" s="63"/>
+      <c r="AB4" s="63"/>
+      <c r="AC4" s="63"/>
+      <c r="AD4" s="63"/>
     </row>
     <row r="5" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B5" s="56" t="s">
+      <c r="B5" s="67" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="56"/>
-      <c r="Z5" s="52"/>
-      <c r="AA5" s="52"/>
-      <c r="AB5" s="52"/>
-      <c r="AC5" s="52"/>
-      <c r="AD5" s="52"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="Z5" s="63"/>
+      <c r="AA5" s="63"/>
+      <c r="AB5" s="63"/>
+      <c r="AC5" s="63"/>
+      <c r="AD5" s="63"/>
     </row>
     <row r="6" spans="2:30" x14ac:dyDescent="0.35">
       <c r="B6" s="24"/>
@@ -7412,37 +7412,37 @@
       <c r="F7" s="24"/>
     </row>
     <row r="8" spans="2:30" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="52" t="s">
+      <c r="B8" s="63" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="52"/>
-      <c r="D8" s="52"/>
-      <c r="E8" s="52"/>
-      <c r="F8" s="52"/>
+      <c r="C8" s="63"/>
+      <c r="D8" s="63"/>
+      <c r="E8" s="63"/>
+      <c r="F8" s="63"/>
     </row>
     <row r="9" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B9" s="52"/>
-      <c r="C9" s="52"/>
-      <c r="D9" s="52"/>
-      <c r="E9" s="52"/>
-      <c r="F9" s="52"/>
+      <c r="B9" s="63"/>
+      <c r="C9" s="63"/>
+      <c r="D9" s="63"/>
+      <c r="E9" s="63"/>
+      <c r="F9" s="63"/>
     </row>
     <row r="10" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B10" s="52"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="52"/>
+      <c r="B10" s="63"/>
+      <c r="C10" s="63"/>
+      <c r="D10" s="63"/>
+      <c r="E10" s="63"/>
+      <c r="F10" s="63"/>
     </row>
     <row r="11" spans="2:30" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B11" s="53" t="str">
+      <c r="B11" s="64" t="str">
         <f>HYPERLINK("https://betrue3d.dk/rpi-and-duet-3-why-and-how/?fbclid=IwAR16IzLQhu4W4G6IMp81qFp3ousTRf1AjmVV-9iawk4osm4pF1tQDGAXfwg","-&gt; Duet &amp; Raspberry Pi &lt;-")</f>
         <v>-&gt; Duet &amp; Raspberry Pi &lt;-</v>
       </c>
-      <c r="C11" s="54"/>
-      <c r="D11" s="54"/>
-      <c r="E11" s="54"/>
-      <c r="F11" s="54"/>
+      <c r="C11" s="65"/>
+      <c r="D11" s="65"/>
+      <c r="E11" s="65"/>
+      <c r="F11" s="65"/>
     </row>
     <row r="12" spans="2:30" x14ac:dyDescent="0.35">
       <c r="B12" s="31"/>
@@ -7457,63 +7457,63 @@
       <c r="D13" s="24"/>
       <c r="E13" s="24"/>
       <c r="F13" s="24"/>
-      <c r="Z13" s="50" t="s">
+      <c r="Z13" s="61" t="s">
         <v>40</v>
       </c>
-      <c r="AA13" s="50"/>
-      <c r="AB13" s="50"/>
-      <c r="AC13" s="50"/>
-      <c r="AD13" s="50"/>
+      <c r="AA13" s="61"/>
+      <c r="AB13" s="61"/>
+      <c r="AC13" s="61"/>
+      <c r="AD13" s="61"/>
     </row>
     <row r="14" spans="2:30" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="52" t="s">
+      <c r="B14" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="52"/>
-      <c r="D14" s="52"/>
-      <c r="E14" s="52"/>
-      <c r="F14" s="52"/>
-      <c r="Z14" s="50"/>
-      <c r="AA14" s="50"/>
-      <c r="AB14" s="50"/>
-      <c r="AC14" s="50"/>
-      <c r="AD14" s="50"/>
+      <c r="C14" s="63"/>
+      <c r="D14" s="63"/>
+      <c r="E14" s="63"/>
+      <c r="F14" s="63"/>
+      <c r="Z14" s="61"/>
+      <c r="AA14" s="61"/>
+      <c r="AB14" s="61"/>
+      <c r="AC14" s="61"/>
+      <c r="AD14" s="61"/>
     </row>
     <row r="15" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B15" s="52"/>
-      <c r="C15" s="52"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="52"/>
-      <c r="F15" s="52"/>
-      <c r="Z15" s="50"/>
-      <c r="AA15" s="50"/>
-      <c r="AB15" s="50"/>
-      <c r="AC15" s="50"/>
-      <c r="AD15" s="50"/>
+      <c r="B15" s="63"/>
+      <c r="C15" s="63"/>
+      <c r="D15" s="63"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="63"/>
+      <c r="Z15" s="61"/>
+      <c r="AA15" s="61"/>
+      <c r="AB15" s="61"/>
+      <c r="AC15" s="61"/>
+      <c r="AD15" s="61"/>
     </row>
     <row r="16" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B16" s="52"/>
-      <c r="C16" s="52"/>
-      <c r="D16" s="52"/>
-      <c r="E16" s="52"/>
-      <c r="F16" s="52"/>
-      <c r="Z16" s="50"/>
-      <c r="AA16" s="50"/>
-      <c r="AB16" s="50"/>
-      <c r="AC16" s="50"/>
-      <c r="AD16" s="50"/>
+      <c r="B16" s="63"/>
+      <c r="C16" s="63"/>
+      <c r="D16" s="63"/>
+      <c r="E16" s="63"/>
+      <c r="F16" s="63"/>
+      <c r="Z16" s="61"/>
+      <c r="AA16" s="61"/>
+      <c r="AB16" s="61"/>
+      <c r="AC16" s="61"/>
+      <c r="AD16" s="61"/>
     </row>
     <row r="17" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B17" s="52"/>
-      <c r="C17" s="52"/>
-      <c r="D17" s="52"/>
-      <c r="E17" s="52"/>
-      <c r="F17" s="52"/>
-      <c r="Z17" s="50"/>
-      <c r="AA17" s="50"/>
-      <c r="AB17" s="50"/>
-      <c r="AC17" s="50"/>
-      <c r="AD17" s="50"/>
+      <c r="B17" s="63"/>
+      <c r="C17" s="63"/>
+      <c r="D17" s="63"/>
+      <c r="E17" s="63"/>
+      <c r="F17" s="63"/>
+      <c r="Z17" s="61"/>
+      <c r="AA17" s="61"/>
+      <c r="AB17" s="61"/>
+      <c r="AC17" s="61"/>
+      <c r="AD17" s="61"/>
     </row>
     <row r="18" spans="2:30" x14ac:dyDescent="0.35">
       <c r="B18" s="24"/>
@@ -7521,11 +7521,11 @@
       <c r="D18" s="24"/>
       <c r="E18" s="24"/>
       <c r="F18" s="24"/>
-      <c r="Z18" s="50"/>
-      <c r="AA18" s="50"/>
-      <c r="AB18" s="50"/>
-      <c r="AC18" s="50"/>
-      <c r="AD18" s="50"/>
+      <c r="Z18" s="61"/>
+      <c r="AA18" s="61"/>
+      <c r="AB18" s="61"/>
+      <c r="AC18" s="61"/>
+      <c r="AD18" s="61"/>
     </row>
     <row r="19" spans="2:30" x14ac:dyDescent="0.35">
       <c r="B19" s="24"/>
@@ -7533,263 +7533,263 @@
       <c r="D19" s="24"/>
       <c r="E19" s="24"/>
       <c r="F19" s="24"/>
-      <c r="Z19" s="50"/>
-      <c r="AA19" s="50"/>
-      <c r="AB19" s="50"/>
-      <c r="AC19" s="50"/>
-      <c r="AD19" s="50"/>
+      <c r="Z19" s="61"/>
+      <c r="AA19" s="61"/>
+      <c r="AB19" s="61"/>
+      <c r="AC19" s="61"/>
+      <c r="AD19" s="61"/>
     </row>
     <row r="20" spans="2:30" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="52" t="s">
+      <c r="B20" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="52"/>
-      <c r="D20" s="52"/>
-      <c r="E20" s="52"/>
-      <c r="F20" s="52"/>
-      <c r="Z20" s="50"/>
-      <c r="AA20" s="50"/>
-      <c r="AB20" s="50"/>
-      <c r="AC20" s="50"/>
-      <c r="AD20" s="50"/>
+      <c r="C20" s="63"/>
+      <c r="D20" s="63"/>
+      <c r="E20" s="63"/>
+      <c r="F20" s="63"/>
+      <c r="Z20" s="61"/>
+      <c r="AA20" s="61"/>
+      <c r="AB20" s="61"/>
+      <c r="AC20" s="61"/>
+      <c r="AD20" s="61"/>
     </row>
     <row r="21" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B21" s="52"/>
-      <c r="C21" s="52"/>
-      <c r="D21" s="52"/>
-      <c r="E21" s="52"/>
-      <c r="F21" s="52"/>
-      <c r="Z21" s="50"/>
-      <c r="AA21" s="50"/>
-      <c r="AB21" s="50"/>
-      <c r="AC21" s="50"/>
-      <c r="AD21" s="50"/>
+      <c r="B21" s="63"/>
+      <c r="C21" s="63"/>
+      <c r="D21" s="63"/>
+      <c r="E21" s="63"/>
+      <c r="F21" s="63"/>
+      <c r="Z21" s="61"/>
+      <c r="AA21" s="61"/>
+      <c r="AB21" s="61"/>
+      <c r="AC21" s="61"/>
+      <c r="AD21" s="61"/>
     </row>
     <row r="22" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B22" s="52"/>
-      <c r="C22" s="52"/>
-      <c r="D22" s="52"/>
-      <c r="E22" s="52"/>
-      <c r="F22" s="52"/>
-      <c r="Z22" s="50"/>
-      <c r="AA22" s="50"/>
-      <c r="AB22" s="50"/>
-      <c r="AC22" s="50"/>
-      <c r="AD22" s="50"/>
+      <c r="B22" s="63"/>
+      <c r="C22" s="63"/>
+      <c r="D22" s="63"/>
+      <c r="E22" s="63"/>
+      <c r="F22" s="63"/>
+      <c r="Z22" s="61"/>
+      <c r="AA22" s="61"/>
+      <c r="AB22" s="61"/>
+      <c r="AC22" s="61"/>
+      <c r="AD22" s="61"/>
     </row>
     <row r="23" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B23" s="52"/>
-      <c r="C23" s="52"/>
-      <c r="D23" s="52"/>
-      <c r="E23" s="52"/>
-      <c r="F23" s="52"/>
-      <c r="Z23" s="50"/>
-      <c r="AA23" s="50"/>
-      <c r="AB23" s="50"/>
-      <c r="AC23" s="50"/>
-      <c r="AD23" s="50"/>
+      <c r="B23" s="63"/>
+      <c r="C23" s="63"/>
+      <c r="D23" s="63"/>
+      <c r="E23" s="63"/>
+      <c r="F23" s="63"/>
+      <c r="Z23" s="61"/>
+      <c r="AA23" s="61"/>
+      <c r="AB23" s="61"/>
+      <c r="AC23" s="61"/>
+      <c r="AD23" s="61"/>
     </row>
     <row r="24" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B24" s="52"/>
-      <c r="C24" s="52"/>
-      <c r="D24" s="52"/>
-      <c r="E24" s="52"/>
-      <c r="F24" s="52"/>
-      <c r="Z24" s="50"/>
-      <c r="AA24" s="50"/>
-      <c r="AB24" s="50"/>
-      <c r="AC24" s="50"/>
-      <c r="AD24" s="50"/>
+      <c r="B24" s="63"/>
+      <c r="C24" s="63"/>
+      <c r="D24" s="63"/>
+      <c r="E24" s="63"/>
+      <c r="F24" s="63"/>
+      <c r="Z24" s="61"/>
+      <c r="AA24" s="61"/>
+      <c r="AB24" s="61"/>
+      <c r="AC24" s="61"/>
+      <c r="AD24" s="61"/>
     </row>
     <row r="25" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B25" s="52"/>
-      <c r="C25" s="52"/>
-      <c r="D25" s="52"/>
-      <c r="E25" s="52"/>
-      <c r="F25" s="52"/>
-      <c r="Z25" s="50"/>
-      <c r="AA25" s="50"/>
-      <c r="AB25" s="50"/>
-      <c r="AC25" s="50"/>
-      <c r="AD25" s="50"/>
+      <c r="B25" s="63"/>
+      <c r="C25" s="63"/>
+      <c r="D25" s="63"/>
+      <c r="E25" s="63"/>
+      <c r="F25" s="63"/>
+      <c r="Z25" s="61"/>
+      <c r="AA25" s="61"/>
+      <c r="AB25" s="61"/>
+      <c r="AC25" s="61"/>
+      <c r="AD25" s="61"/>
     </row>
     <row r="26" spans="2:30" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B26" s="52"/>
-      <c r="C26" s="52"/>
-      <c r="D26" s="52"/>
-      <c r="E26" s="52"/>
-      <c r="F26" s="52"/>
-      <c r="Z26" s="55" t="str">
+      <c r="B26" s="63"/>
+      <c r="C26" s="63"/>
+      <c r="D26" s="63"/>
+      <c r="E26" s="63"/>
+      <c r="F26" s="63"/>
+      <c r="Z26" s="66" t="str">
         <f>HYPERLINK("https://duet3d.dozuki.com/Wiki/Gcode#Section_M911_Configure_auto_save_on_loss_of_power","Read more: -&gt; M911 Gcode &lt;-")</f>
         <v>Read more: -&gt; M911 Gcode &lt;-</v>
       </c>
-      <c r="AA26" s="55"/>
-      <c r="AB26" s="55"/>
-      <c r="AC26" s="55"/>
-      <c r="AD26" s="55"/>
+      <c r="AA26" s="66"/>
+      <c r="AB26" s="66"/>
+      <c r="AC26" s="66"/>
+      <c r="AD26" s="66"/>
     </row>
     <row r="29" spans="2:30" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="51" t="s">
+      <c r="B29" s="62" t="s">
         <v>43</v>
       </c>
-      <c r="C29" s="51"/>
-      <c r="D29" s="51"/>
-      <c r="E29" s="51"/>
-      <c r="F29" s="51"/>
-      <c r="Z29" s="57" t="s">
+      <c r="C29" s="62"/>
+      <c r="D29" s="62"/>
+      <c r="E29" s="62"/>
+      <c r="F29" s="62"/>
+      <c r="Z29" s="68" t="s">
         <v>45</v>
       </c>
-      <c r="AA29" s="57"/>
-      <c r="AB29" s="57"/>
-      <c r="AC29" s="57"/>
-      <c r="AD29" s="57"/>
+      <c r="AA29" s="68"/>
+      <c r="AB29" s="68"/>
+      <c r="AC29" s="68"/>
+      <c r="AD29" s="68"/>
     </row>
     <row r="30" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B30" s="51"/>
-      <c r="C30" s="51"/>
-      <c r="D30" s="51"/>
-      <c r="E30" s="51"/>
-      <c r="F30" s="51"/>
-      <c r="Z30" s="57"/>
-      <c r="AA30" s="57"/>
-      <c r="AB30" s="57"/>
-      <c r="AC30" s="57"/>
-      <c r="AD30" s="57"/>
+      <c r="B30" s="62"/>
+      <c r="C30" s="62"/>
+      <c r="D30" s="62"/>
+      <c r="E30" s="62"/>
+      <c r="F30" s="62"/>
+      <c r="Z30" s="68"/>
+      <c r="AA30" s="68"/>
+      <c r="AB30" s="68"/>
+      <c r="AC30" s="68"/>
+      <c r="AD30" s="68"/>
     </row>
     <row r="31" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B31" s="51"/>
-      <c r="C31" s="51"/>
-      <c r="D31" s="51"/>
-      <c r="E31" s="51"/>
-      <c r="F31" s="51"/>
-      <c r="Z31" s="57"/>
-      <c r="AA31" s="57"/>
-      <c r="AB31" s="57"/>
-      <c r="AC31" s="57"/>
-      <c r="AD31" s="57"/>
+      <c r="B31" s="62"/>
+      <c r="C31" s="62"/>
+      <c r="D31" s="62"/>
+      <c r="E31" s="62"/>
+      <c r="F31" s="62"/>
+      <c r="Z31" s="68"/>
+      <c r="AA31" s="68"/>
+      <c r="AB31" s="68"/>
+      <c r="AC31" s="68"/>
+      <c r="AD31" s="68"/>
     </row>
     <row r="32" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="Z32" s="57"/>
-      <c r="AA32" s="57"/>
-      <c r="AB32" s="57"/>
-      <c r="AC32" s="57"/>
-      <c r="AD32" s="57"/>
+      <c r="Z32" s="68"/>
+      <c r="AA32" s="68"/>
+      <c r="AB32" s="68"/>
+      <c r="AC32" s="68"/>
+      <c r="AD32" s="68"/>
     </row>
     <row r="33" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="Z33" s="57"/>
-      <c r="AA33" s="57"/>
-      <c r="AB33" s="57"/>
-      <c r="AC33" s="57"/>
-      <c r="AD33" s="57"/>
+      <c r="Z33" s="68"/>
+      <c r="AA33" s="68"/>
+      <c r="AB33" s="68"/>
+      <c r="AC33" s="68"/>
+      <c r="AD33" s="68"/>
     </row>
     <row r="34" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B34" s="50" t="s">
+      <c r="B34" s="61" t="s">
         <v>46</v>
       </c>
-      <c r="C34" s="50"/>
-      <c r="D34" s="50"/>
-      <c r="E34" s="50"/>
-      <c r="F34" s="50"/>
-      <c r="Z34" s="57"/>
-      <c r="AA34" s="57"/>
-      <c r="AB34" s="57"/>
-      <c r="AC34" s="57"/>
-      <c r="AD34" s="57"/>
+      <c r="C34" s="61"/>
+      <c r="D34" s="61"/>
+      <c r="E34" s="61"/>
+      <c r="F34" s="61"/>
+      <c r="Z34" s="68"/>
+      <c r="AA34" s="68"/>
+      <c r="AB34" s="68"/>
+      <c r="AC34" s="68"/>
+      <c r="AD34" s="68"/>
     </row>
     <row r="35" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B35" s="50"/>
-      <c r="C35" s="50"/>
-      <c r="D35" s="50"/>
-      <c r="E35" s="50"/>
-      <c r="F35" s="50"/>
-      <c r="Z35" s="57"/>
-      <c r="AA35" s="57"/>
-      <c r="AB35" s="57"/>
-      <c r="AC35" s="57"/>
-      <c r="AD35" s="57"/>
+      <c r="B35" s="61"/>
+      <c r="C35" s="61"/>
+      <c r="D35" s="61"/>
+      <c r="E35" s="61"/>
+      <c r="F35" s="61"/>
+      <c r="Z35" s="68"/>
+      <c r="AA35" s="68"/>
+      <c r="AB35" s="68"/>
+      <c r="AC35" s="68"/>
+      <c r="AD35" s="68"/>
     </row>
     <row r="36" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B36" s="50"/>
-      <c r="C36" s="50"/>
-      <c r="D36" s="50"/>
-      <c r="E36" s="50"/>
-      <c r="F36" s="50"/>
-      <c r="Z36" s="57"/>
-      <c r="AA36" s="57"/>
-      <c r="AB36" s="57"/>
-      <c r="AC36" s="57"/>
-      <c r="AD36" s="57"/>
+      <c r="B36" s="61"/>
+      <c r="C36" s="61"/>
+      <c r="D36" s="61"/>
+      <c r="E36" s="61"/>
+      <c r="F36" s="61"/>
+      <c r="Z36" s="68"/>
+      <c r="AA36" s="68"/>
+      <c r="AB36" s="68"/>
+      <c r="AC36" s="68"/>
+      <c r="AD36" s="68"/>
     </row>
     <row r="37" spans="2:30" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="50"/>
-      <c r="C37" s="50"/>
-      <c r="D37" s="50"/>
-      <c r="E37" s="50"/>
-      <c r="F37" s="50"/>
-      <c r="Z37" s="57"/>
-      <c r="AA37" s="57"/>
-      <c r="AB37" s="57"/>
-      <c r="AC37" s="57"/>
-      <c r="AD37" s="57"/>
+      <c r="B37" s="61"/>
+      <c r="C37" s="61"/>
+      <c r="D37" s="61"/>
+      <c r="E37" s="61"/>
+      <c r="F37" s="61"/>
+      <c r="Z37" s="68"/>
+      <c r="AA37" s="68"/>
+      <c r="AB37" s="68"/>
+      <c r="AC37" s="68"/>
+      <c r="AD37" s="68"/>
     </row>
     <row r="38" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="Z38" s="57"/>
-      <c r="AA38" s="57"/>
-      <c r="AB38" s="57"/>
-      <c r="AC38" s="57"/>
-      <c r="AD38" s="57"/>
+      <c r="Z38" s="68"/>
+      <c r="AA38" s="68"/>
+      <c r="AB38" s="68"/>
+      <c r="AC38" s="68"/>
+      <c r="AD38" s="68"/>
     </row>
     <row r="39" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="Z39" s="57"/>
-      <c r="AA39" s="57"/>
-      <c r="AB39" s="57"/>
-      <c r="AC39" s="57"/>
-      <c r="AD39" s="57"/>
+      <c r="Z39" s="68"/>
+      <c r="AA39" s="68"/>
+      <c r="AB39" s="68"/>
+      <c r="AC39" s="68"/>
+      <c r="AD39" s="68"/>
     </row>
     <row r="40" spans="2:30" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="50" t="s">
+      <c r="B40" s="61" t="s">
         <v>47</v>
       </c>
-      <c r="C40" s="50"/>
-      <c r="D40" s="50"/>
-      <c r="E40" s="50"/>
-      <c r="F40" s="50"/>
-      <c r="Z40" s="57"/>
-      <c r="AA40" s="57"/>
-      <c r="AB40" s="57"/>
-      <c r="AC40" s="57"/>
-      <c r="AD40" s="57"/>
+      <c r="C40" s="61"/>
+      <c r="D40" s="61"/>
+      <c r="E40" s="61"/>
+      <c r="F40" s="61"/>
+      <c r="Z40" s="68"/>
+      <c r="AA40" s="68"/>
+      <c r="AB40" s="68"/>
+      <c r="AC40" s="68"/>
+      <c r="AD40" s="68"/>
     </row>
     <row r="41" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B41" s="50"/>
-      <c r="C41" s="50"/>
-      <c r="D41" s="50"/>
-      <c r="E41" s="50"/>
-      <c r="F41" s="50"/>
-      <c r="Z41" s="57"/>
-      <c r="AA41" s="57"/>
-      <c r="AB41" s="57"/>
-      <c r="AC41" s="57"/>
-      <c r="AD41" s="57"/>
+      <c r="B41" s="61"/>
+      <c r="C41" s="61"/>
+      <c r="D41" s="61"/>
+      <c r="E41" s="61"/>
+      <c r="F41" s="61"/>
+      <c r="Z41" s="68"/>
+      <c r="AA41" s="68"/>
+      <c r="AB41" s="68"/>
+      <c r="AC41" s="68"/>
+      <c r="AD41" s="68"/>
     </row>
     <row r="42" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B42" s="50"/>
-      <c r="C42" s="50"/>
-      <c r="D42" s="50"/>
-      <c r="E42" s="50"/>
-      <c r="F42" s="50"/>
-      <c r="Z42" s="57"/>
-      <c r="AA42" s="57"/>
-      <c r="AB42" s="57"/>
-      <c r="AC42" s="57"/>
-      <c r="AD42" s="57"/>
+      <c r="B42" s="61"/>
+      <c r="C42" s="61"/>
+      <c r="D42" s="61"/>
+      <c r="E42" s="61"/>
+      <c r="F42" s="61"/>
+      <c r="Z42" s="68"/>
+      <c r="AA42" s="68"/>
+      <c r="AB42" s="68"/>
+      <c r="AC42" s="68"/>
+      <c r="AD42" s="68"/>
     </row>
     <row r="43" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B43" s="50"/>
-      <c r="C43" s="50"/>
-      <c r="D43" s="50"/>
-      <c r="E43" s="50"/>
-      <c r="F43" s="50"/>
+      <c r="B43" s="61"/>
+      <c r="C43" s="61"/>
+      <c r="D43" s="61"/>
+      <c r="E43" s="61"/>
+      <c r="F43" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -7837,27 +7837,27 @@
   </cols>
   <sheetData>
     <row r="6" spans="26:30" x14ac:dyDescent="0.35">
-      <c r="Z6" s="58" t="s">
+      <c r="Z6" s="69" t="s">
         <v>57</v>
       </c>
-      <c r="AA6" s="58"/>
-      <c r="AB6" s="58"/>
-      <c r="AC6" s="58"/>
-      <c r="AD6" s="58"/>
+      <c r="AA6" s="69"/>
+      <c r="AB6" s="69"/>
+      <c r="AC6" s="69"/>
+      <c r="AD6" s="69"/>
     </row>
     <row r="7" spans="26:30" x14ac:dyDescent="0.35">
-      <c r="Z7" s="58"/>
-      <c r="AA7" s="58"/>
-      <c r="AB7" s="58"/>
-      <c r="AC7" s="58"/>
-      <c r="AD7" s="58"/>
+      <c r="Z7" s="69"/>
+      <c r="AA7" s="69"/>
+      <c r="AB7" s="69"/>
+      <c r="AC7" s="69"/>
+      <c r="AD7" s="69"/>
     </row>
     <row r="8" spans="26:30" x14ac:dyDescent="0.35">
-      <c r="Z8" s="58"/>
-      <c r="AA8" s="58"/>
-      <c r="AB8" s="58"/>
-      <c r="AC8" s="58"/>
-      <c r="AD8" s="58"/>
+      <c r="Z8" s="69"/>
+      <c r="AA8" s="69"/>
+      <c r="AB8" s="69"/>
+      <c r="AC8" s="69"/>
+      <c r="AD8" s="69"/>
     </row>
     <row r="21" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="22" spans="2:7" x14ac:dyDescent="0.35">
@@ -7899,65 +7899,65 @@
     <row r="27" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B27" s="23"/>
       <c r="C27" s="25"/>
-      <c r="E27" s="50" t="s">
+      <c r="E27" s="61" t="s">
         <v>56</v>
       </c>
-      <c r="F27" s="50"/>
-      <c r="G27" s="50"/>
+      <c r="F27" s="61"/>
+      <c r="G27" s="61"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B28" s="23"/>
       <c r="C28" s="25"/>
-      <c r="E28" s="50"/>
-      <c r="F28" s="50"/>
-      <c r="G28" s="50"/>
+      <c r="E28" s="61"/>
+      <c r="F28" s="61"/>
+      <c r="G28" s="61"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B29" s="23"/>
       <c r="C29" s="25"/>
-      <c r="E29" s="50"/>
-      <c r="F29" s="50"/>
-      <c r="G29" s="50"/>
+      <c r="E29" s="61"/>
+      <c r="F29" s="61"/>
+      <c r="G29" s="61"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B30" s="23"/>
       <c r="C30" s="25"/>
-      <c r="E30" s="50"/>
-      <c r="F30" s="50"/>
-      <c r="G30" s="50"/>
+      <c r="E30" s="61"/>
+      <c r="F30" s="61"/>
+      <c r="G30" s="61"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B31" s="23"/>
       <c r="C31" s="25"/>
-      <c r="E31" s="50"/>
-      <c r="F31" s="50"/>
-      <c r="G31" s="50"/>
+      <c r="E31" s="61"/>
+      <c r="F31" s="61"/>
+      <c r="G31" s="61"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B32" s="23"/>
       <c r="C32" s="25"/>
-      <c r="E32" s="50"/>
-      <c r="F32" s="50"/>
-      <c r="G32" s="50"/>
+      <c r="E32" s="61"/>
+      <c r="F32" s="61"/>
+      <c r="G32" s="61"/>
     </row>
     <row r="33" spans="2:30" x14ac:dyDescent="0.35">
       <c r="B33" s="23"/>
       <c r="C33" s="25"/>
-      <c r="E33" s="50"/>
-      <c r="F33" s="50"/>
-      <c r="G33" s="50"/>
+      <c r="E33" s="61"/>
+      <c r="F33" s="61"/>
+      <c r="G33" s="61"/>
     </row>
     <row r="34" spans="2:30" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B34" s="36"/>
       <c r="C34" s="27"/>
-      <c r="E34" s="50"/>
-      <c r="F34" s="50"/>
-      <c r="G34" s="50"/>
+      <c r="E34" s="61"/>
+      <c r="F34" s="61"/>
+      <c r="G34" s="61"/>
     </row>
     <row r="35" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="E35" s="50"/>
-      <c r="F35" s="50"/>
-      <c r="G35" s="50"/>
+      <c r="E35" s="61"/>
+      <c r="F35" s="61"/>
+      <c r="G35" s="61"/>
     </row>
     <row r="38" spans="2:30" x14ac:dyDescent="0.35">
       <c r="Z38" s="37"/>
@@ -8020,7 +8020,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AG11" sqref="AG11"/>
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8152,10 +8152,10 @@
   <sheetPr>
     <tabColor rgb="FFFF00FF"/>
   </sheetPr>
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8166,14 +8166,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="49" t="s">
+      <c r="C1" s="59"/>
+      <c r="D1" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="49"/>
+      <c r="E1" s="60"/>
       <c r="I1" t="s">
         <v>15</v>
       </c>
@@ -8326,11 +8326,11 @@
         <v>415</v>
       </c>
       <c r="I7">
-        <f t="shared" ref="I7:I16" si="0">H7-H6+I6</f>
+        <f t="shared" ref="I7:I9" si="0">H7-H6+I6</f>
         <v>452.41800000000001</v>
       </c>
       <c r="J7">
-        <f t="shared" ref="J7:J16" si="1">H7-H6+J6</f>
+        <f t="shared" ref="J7:J9" si="1">H7-H6+J6</f>
         <v>428.21</v>
       </c>
     </row>
@@ -8407,15 +8407,15 @@
         <v>46</v>
       </c>
       <c r="H10">
-        <v>515</v>
+        <v>500</v>
       </c>
       <c r="I10">
-        <f t="shared" si="0"/>
-        <v>552.41800000000001</v>
+        <f>H10-H9+I9</f>
+        <v>537.41800000000001</v>
       </c>
       <c r="J10">
-        <f t="shared" si="1"/>
-        <v>528.21</v>
+        <f>H10-H9+J9</f>
+        <v>513.21</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
@@ -8435,79 +8435,92 @@
         <v>5.21</v>
       </c>
       <c r="H11">
-        <v>565</v>
+        <v>515</v>
       </c>
       <c r="I11">
-        <f t="shared" si="0"/>
-        <v>602.41800000000001</v>
+        <f>H11-H9+I9</f>
+        <v>552.41800000000001</v>
       </c>
       <c r="J11">
-        <f t="shared" si="1"/>
-        <v>578.21</v>
+        <f>H11-H9+J9</f>
+        <v>528.21</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="H12">
-        <v>615</v>
+        <v>565</v>
       </c>
       <c r="I12">
-        <f t="shared" si="0"/>
-        <v>652.41800000000001</v>
+        <f>H12-H11+I11</f>
+        <v>602.41800000000001</v>
       </c>
       <c r="J12">
-        <f t="shared" si="1"/>
-        <v>628.21</v>
+        <f>H12-H11+J11</f>
+        <v>578.21</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="H13">
-        <v>665</v>
+        <v>615</v>
       </c>
       <c r="I13">
-        <f t="shared" si="0"/>
-        <v>702.41800000000001</v>
+        <f>H13-H12+I12</f>
+        <v>652.41800000000001</v>
       </c>
       <c r="J13">
-        <f t="shared" si="1"/>
-        <v>678.21</v>
+        <f>H13-H12+J12</f>
+        <v>628.21</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="H14">
-        <v>715</v>
+        <v>665</v>
       </c>
       <c r="I14">
-        <f t="shared" si="0"/>
-        <v>752.41800000000001</v>
+        <f>H14-H13+I13</f>
+        <v>702.41800000000001</v>
       </c>
       <c r="J14">
-        <f t="shared" si="1"/>
-        <v>728.21</v>
+        <f>H14-H13+J13</f>
+        <v>678.21</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="H15">
-        <v>765</v>
+        <v>715</v>
       </c>
       <c r="I15">
-        <f t="shared" si="0"/>
-        <v>802.41800000000001</v>
+        <f>H15-H14+I14</f>
+        <v>752.41800000000001</v>
       </c>
       <c r="J15">
-        <f t="shared" si="1"/>
-        <v>778.21</v>
+        <f>H15-H14+J14</f>
+        <v>728.21</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="H16">
+        <v>765</v>
+      </c>
+      <c r="I16">
+        <f>H16-H15+I15</f>
+        <v>802.41800000000001</v>
+      </c>
+      <c r="J16">
+        <f>H16-H15+J15</f>
+        <v>778.21</v>
+      </c>
+    </row>
+    <row r="17" spans="8:10" x14ac:dyDescent="0.35">
+      <c r="H17">
         <v>815</v>
       </c>
-      <c r="I16">
-        <f t="shared" si="0"/>
+      <c r="I17">
+        <f>H17-H16+I16</f>
         <v>852.41800000000001</v>
       </c>
-      <c r="J16">
-        <f t="shared" si="1"/>
+      <c r="J17">
+        <f>H17-H16+J16</f>
         <v>828.21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
POS8 pn alternative and source added
</commit_message>
<xml_diff>
--- a/FirmWareSettings.xlsx
+++ b/FirmWareSettings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivi\OneDrive\Documents\GitHub\HevORT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D68B6714-F2ED-4709-AC29-15A62BF7BF8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBC8A906-A474-4434-974E-CB7F17FE7F10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{509C0CBF-6515-4E03-BB96-B231BA0137C3}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="67">
   <si>
     <t>PRINT_HEAD</t>
   </si>
@@ -491,6 +491,9 @@
   </si>
   <si>
     <t>KLIPPER (for printer.cfg file)</t>
+  </si>
+  <si>
+    <t>M671 X-38.188:230.521:499.23 Y-20.717:492.493:-20.717 S50</t>
   </si>
 </sst>
 </file>
@@ -6994,7 +6997,7 @@
   <dimension ref="A1:U50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A20" sqref="A20:B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7213,7 +7216,9 @@
       <c r="B25" s="45"/>
     </row>
     <row r="27" spans="1:19" ht="28.5" x14ac:dyDescent="0.65">
-      <c r="A27" s="5"/>
+      <c r="A27" s="5" t="s">
+        <v>66</v>
+      </c>
       <c r="D27" t="s">
         <v>18</v>
       </c>
@@ -8451,11 +8456,11 @@
         <v>565</v>
       </c>
       <c r="I12">
-        <f>H12-H11+I11</f>
+        <f t="shared" ref="I12:I17" si="2">H12-H11+I11</f>
         <v>602.41800000000001</v>
       </c>
       <c r="J12">
-        <f>H12-H11+J11</f>
+        <f t="shared" ref="J12:J17" si="3">H12-H11+J11</f>
         <v>578.21</v>
       </c>
     </row>
@@ -8464,11 +8469,11 @@
         <v>615</v>
       </c>
       <c r="I13">
-        <f>H13-H12+I12</f>
+        <f t="shared" si="2"/>
         <v>652.41800000000001</v>
       </c>
       <c r="J13">
-        <f>H13-H12+J12</f>
+        <f t="shared" si="3"/>
         <v>628.21</v>
       </c>
     </row>
@@ -8477,11 +8482,11 @@
         <v>665</v>
       </c>
       <c r="I14">
-        <f>H14-H13+I13</f>
+        <f t="shared" si="2"/>
         <v>702.41800000000001</v>
       </c>
       <c r="J14">
-        <f>H14-H13+J13</f>
+        <f t="shared" si="3"/>
         <v>678.21</v>
       </c>
     </row>
@@ -8490,11 +8495,11 @@
         <v>715</v>
       </c>
       <c r="I15">
-        <f>H15-H14+I14</f>
+        <f t="shared" si="2"/>
         <v>752.41800000000001</v>
       </c>
       <c r="J15">
-        <f>H15-H14+J14</f>
+        <f t="shared" si="3"/>
         <v>728.21</v>
       </c>
     </row>
@@ -8503,11 +8508,11 @@
         <v>765</v>
       </c>
       <c r="I16">
-        <f>H16-H15+I15</f>
+        <f t="shared" si="2"/>
         <v>802.41800000000001</v>
       </c>
       <c r="J16">
-        <f>H16-H15+J15</f>
+        <f t="shared" si="3"/>
         <v>778.21</v>
       </c>
     </row>
@@ -8516,11 +8521,11 @@
         <v>815</v>
       </c>
       <c r="I17">
-        <f>H17-H16+I16</f>
+        <f t="shared" si="2"/>
         <v>852.41800000000001</v>
       </c>
       <c r="J17">
-        <f>H17-H16+J16</f>
+        <f t="shared" si="3"/>
         <v>828.21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
BLtouch for Hextrudort iOffset corrected
</commit_message>
<xml_diff>
--- a/FirmWareSettings.xlsx
+++ b/FirmWareSettings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivi\OneDrive\Documents\GitHub\HevORT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9AB0BA3-A3DF-4972-9EEA-3959B65FB077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17C03BAE-15E9-435C-9D64-12516CB2071A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="789" xr2:uid="{509C0CBF-6515-4E03-BB96-B231BA0137C3}"/>
   </bookViews>
@@ -1137,6 +1137,22 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1173,6 +1189,9 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1199,25 +1218,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -7191,7 +7191,7 @@
   <dimension ref="A1:U51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7228,10 +7228,10 @@
       <c r="C2" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="41" t="s">
+      <c r="I2" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="42"/>
+      <c r="J2" s="48"/>
     </row>
     <row r="3" spans="1:10" ht="26" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
@@ -7243,8 +7243,8 @@
       <c r="C3" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="43"/>
-      <c r="J3" s="44"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="50"/>
     </row>
     <row r="4" spans="1:10" ht="26" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
@@ -7256,14 +7256,14 @@
       <c r="C4" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="43"/>
-      <c r="J4" s="44"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="50"/>
     </row>
     <row r="5" spans="1:10" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="I5" s="47" t="s">
+      <c r="I5" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="J5" s="48"/>
+      <c r="J5" s="54"/>
     </row>
     <row r="6" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A6" s="10" t="s">
@@ -7374,7 +7374,7 @@
     <row r="18" spans="1:19" ht="21.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="40" t="str">
         <f>"G31 P500 X"&amp;VLOOKUP(B4,Table1[],4,0) &amp; " Y"&amp; VLOOKUP(B4,Table1[],5,0) &amp; " Z[measured via Paper technique]"</f>
-        <v>G31 P500 X22.775 Y8.706 Z[measured via Paper technique]</v>
+        <v>G31 P500 X22.775 Y-8.706 Z[measured via Paper technique]</v>
       </c>
       <c r="B18" s="26"/>
       <c r="C18" s="26"/>
@@ -7384,7 +7384,7 @@
     </row>
     <row r="20" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="21" spans="1:19" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="64" t="s">
+      <c r="A21" s="42" t="s">
         <v>64</v>
       </c>
       <c r="B21" s="22"/>
@@ -7402,21 +7402,21 @@
       <c r="B23" s="25"/>
     </row>
     <row r="24" spans="1:19" ht="21" x14ac:dyDescent="0.5">
-      <c r="A24" s="65" t="str">
+      <c r="A24" s="43" t="str">
         <f>B42&amp;","&amp;C42</f>
         <v>-16.87,-20.4</v>
       </c>
       <c r="B24" s="25"/>
     </row>
     <row r="25" spans="1:19" ht="21" x14ac:dyDescent="0.5">
-      <c r="A25" s="65" t="str">
+      <c r="A25" s="43" t="str">
         <f>I7&amp;","&amp;J7</f>
         <v>259.339,507.81</v>
       </c>
       <c r="B25" s="25"/>
     </row>
     <row r="26" spans="1:19" ht="21" x14ac:dyDescent="0.5">
-      <c r="A26" s="65" t="str">
+      <c r="A26" s="43" t="str">
         <f>T42&amp;","&amp;U42</f>
         <v>535.548,-20.4</v>
       </c>
@@ -7452,28 +7452,28 @@
       <c r="B30" s="25"/>
     </row>
     <row r="31" spans="1:19" ht="21" x14ac:dyDescent="0.5">
-      <c r="A31" s="65" t="s">
+      <c r="A31" s="43" t="s">
         <v>76</v>
       </c>
-      <c r="B31" s="67">
-        <f>VLOOKUP(B4,Table1[#All],2,0)</f>
-        <v>28.079000000000001</v>
+      <c r="B31" s="45">
+        <f>VLOOKUP(B4,Table1[#All],4,0)</f>
+        <v>22.774999999999999</v>
       </c>
     </row>
     <row r="32" spans="1:19" ht="21" x14ac:dyDescent="0.5">
-      <c r="A32" s="65" t="s">
+      <c r="A32" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="B32" s="67">
-        <f>VLOOKUP(B4,Table1[#All],3,0)</f>
-        <v>26.9</v>
+      <c r="B32" s="45">
+        <f>VLOOKUP(B4,Table1[#All],5,0)</f>
+        <v>-8.7059999999999995</v>
       </c>
     </row>
     <row r="33" spans="1:21" ht="21.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="66" t="s">
+      <c r="A33" s="44" t="s">
         <v>74</v>
       </c>
-      <c r="B33" s="68">
+      <c r="B33" s="46">
         <v>2</v>
       </c>
     </row>
@@ -7483,42 +7483,42 @@
       </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="B36" s="41" t="s">
+      <c r="B36" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="C36" s="42"/>
-      <c r="T36" s="41" t="s">
+      <c r="C36" s="48"/>
+      <c r="T36" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="U36" s="42"/>
+      <c r="U36" s="48"/>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="B37" s="43"/>
-      <c r="C37" s="44"/>
-      <c r="T37" s="43"/>
-      <c r="U37" s="44"/>
+      <c r="B37" s="49"/>
+      <c r="C37" s="50"/>
+      <c r="T37" s="49"/>
+      <c r="U37" s="50"/>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="B38" s="43"/>
-      <c r="C38" s="44"/>
-      <c r="T38" s="43"/>
-      <c r="U38" s="44"/>
+      <c r="B38" s="49"/>
+      <c r="C38" s="50"/>
+      <c r="T38" s="49"/>
+      <c r="U38" s="50"/>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="B39" s="49"/>
-      <c r="C39" s="50"/>
-      <c r="T39" s="49"/>
-      <c r="U39" s="50"/>
+      <c r="B39" s="55"/>
+      <c r="C39" s="56"/>
+      <c r="T39" s="55"/>
+      <c r="U39" s="56"/>
     </row>
     <row r="40" spans="1:21" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="B40" s="45" t="s">
+      <c r="B40" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="C40" s="46"/>
-      <c r="T40" s="45" t="s">
+      <c r="C40" s="52"/>
+      <c r="T40" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="U40" s="46"/>
+      <c r="U40" s="52"/>
     </row>
     <row r="41" spans="1:21" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B41" s="17" t="s">
@@ -7621,7 +7621,7 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7633,14 +7633,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="52" t="s">
+      <c r="C1" s="57"/>
+      <c r="D1" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="52"/>
+      <c r="E1" s="58"/>
       <c r="I1" t="s">
         <v>15</v>
       </c>
@@ -7899,7 +7899,7 @@
         <v>22.774999999999999</v>
       </c>
       <c r="E11" s="4">
-        <v>5.21</v>
+        <v>-5.21</v>
       </c>
       <c r="H11">
         <v>515</v>
@@ -7927,7 +7927,7 @@
         <v>22.774999999999999</v>
       </c>
       <c r="E12" s="4">
-        <v>8.7059999999999995</v>
+        <v>-8.7059999999999995</v>
       </c>
       <c r="H12">
         <v>565</v>
@@ -7968,10 +7968,10 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B15" s="62" t="s">
+      <c r="B15" s="59" t="s">
         <v>69</v>
       </c>
-      <c r="C15" s="62"/>
+      <c r="C15" s="59"/>
       <c r="H15">
         <v>715</v>
       </c>
@@ -7988,10 +7988,10 @@
       <c r="A16" t="s">
         <v>67</v>
       </c>
-      <c r="B16" s="63" t="s">
+      <c r="B16" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="63" t="s">
+      <c r="C16" s="41" t="s">
         <v>11</v>
       </c>
       <c r="H16">
@@ -8070,46 +8070,46 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:30" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="Z3" s="55" t="s">
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="Z3" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="AA3" s="55"/>
-      <c r="AB3" s="55"/>
-      <c r="AC3" s="55"/>
-      <c r="AD3" s="55"/>
+      <c r="AA3" s="62"/>
+      <c r="AB3" s="62"/>
+      <c r="AC3" s="62"/>
+      <c r="AD3" s="62"/>
     </row>
     <row r="4" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B4" s="55"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="Z4" s="55"/>
-      <c r="AA4" s="55"/>
-      <c r="AB4" s="55"/>
-      <c r="AC4" s="55"/>
-      <c r="AD4" s="55"/>
+      <c r="B4" s="62"/>
+      <c r="C4" s="62"/>
+      <c r="D4" s="62"/>
+      <c r="E4" s="62"/>
+      <c r="F4" s="62"/>
+      <c r="Z4" s="62"/>
+      <c r="AA4" s="62"/>
+      <c r="AB4" s="62"/>
+      <c r="AC4" s="62"/>
+      <c r="AD4" s="62"/>
     </row>
     <row r="5" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="59"/>
-      <c r="D5" s="59"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="59"/>
-      <c r="Z5" s="55"/>
-      <c r="AA5" s="55"/>
-      <c r="AB5" s="55"/>
-      <c r="AC5" s="55"/>
-      <c r="AD5" s="55"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="Z5" s="62"/>
+      <c r="AA5" s="62"/>
+      <c r="AB5" s="62"/>
+      <c r="AC5" s="62"/>
+      <c r="AD5" s="62"/>
     </row>
     <row r="6" spans="2:30" x14ac:dyDescent="0.35">
       <c r="B6" s="24"/>
@@ -8126,37 +8126,37 @@
       <c r="F7" s="24"/>
     </row>
     <row r="8" spans="2:30" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="55" t="s">
+      <c r="B8" s="62" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="55"/>
-      <c r="D8" s="55"/>
-      <c r="E8" s="55"/>
-      <c r="F8" s="55"/>
+      <c r="C8" s="62"/>
+      <c r="D8" s="62"/>
+      <c r="E8" s="62"/>
+      <c r="F8" s="62"/>
     </row>
     <row r="9" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B9" s="55"/>
-      <c r="C9" s="55"/>
-      <c r="D9" s="55"/>
-      <c r="E9" s="55"/>
-      <c r="F9" s="55"/>
+      <c r="B9" s="62"/>
+      <c r="C9" s="62"/>
+      <c r="D9" s="62"/>
+      <c r="E9" s="62"/>
+      <c r="F9" s="62"/>
     </row>
     <row r="10" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B10" s="55"/>
-      <c r="C10" s="55"/>
-      <c r="D10" s="55"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="55"/>
+      <c r="B10" s="62"/>
+      <c r="C10" s="62"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="62"/>
+      <c r="F10" s="62"/>
     </row>
     <row r="11" spans="2:30" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B11" s="56" t="str">
+      <c r="B11" s="63" t="str">
         <f>HYPERLINK("https://betrue3d.dk/rpi-and-duet-3-why-and-how/?fbclid=IwAR16IzLQhu4W4G6IMp81qFp3ousTRf1AjmVV-9iawk4osm4pF1tQDGAXfwg","-&gt; Duet &amp; Raspberry Pi &lt;-")</f>
         <v>-&gt; Duet &amp; Raspberry Pi &lt;-</v>
       </c>
-      <c r="C11" s="57"/>
-      <c r="D11" s="57"/>
-      <c r="E11" s="57"/>
-      <c r="F11" s="57"/>
+      <c r="C11" s="64"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="64"/>
     </row>
     <row r="12" spans="2:30" x14ac:dyDescent="0.35">
       <c r="B12" s="31"/>
@@ -8171,63 +8171,63 @@
       <c r="D13" s="24"/>
       <c r="E13" s="24"/>
       <c r="F13" s="24"/>
-      <c r="Z13" s="53" t="s">
+      <c r="Z13" s="60" t="s">
         <v>40</v>
       </c>
-      <c r="AA13" s="53"/>
-      <c r="AB13" s="53"/>
-      <c r="AC13" s="53"/>
-      <c r="AD13" s="53"/>
+      <c r="AA13" s="60"/>
+      <c r="AB13" s="60"/>
+      <c r="AC13" s="60"/>
+      <c r="AD13" s="60"/>
     </row>
     <row r="14" spans="2:30" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="55" t="s">
+      <c r="B14" s="62" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="55"/>
-      <c r="D14" s="55"/>
-      <c r="E14" s="55"/>
-      <c r="F14" s="55"/>
-      <c r="Z14" s="53"/>
-      <c r="AA14" s="53"/>
-      <c r="AB14" s="53"/>
-      <c r="AC14" s="53"/>
-      <c r="AD14" s="53"/>
+      <c r="C14" s="62"/>
+      <c r="D14" s="62"/>
+      <c r="E14" s="62"/>
+      <c r="F14" s="62"/>
+      <c r="Z14" s="60"/>
+      <c r="AA14" s="60"/>
+      <c r="AB14" s="60"/>
+      <c r="AC14" s="60"/>
+      <c r="AD14" s="60"/>
     </row>
     <row r="15" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B15" s="55"/>
-      <c r="C15" s="55"/>
-      <c r="D15" s="55"/>
-      <c r="E15" s="55"/>
-      <c r="F15" s="55"/>
-      <c r="Z15" s="53"/>
-      <c r="AA15" s="53"/>
-      <c r="AB15" s="53"/>
-      <c r="AC15" s="53"/>
-      <c r="AD15" s="53"/>
+      <c r="B15" s="62"/>
+      <c r="C15" s="62"/>
+      <c r="D15" s="62"/>
+      <c r="E15" s="62"/>
+      <c r="F15" s="62"/>
+      <c r="Z15" s="60"/>
+      <c r="AA15" s="60"/>
+      <c r="AB15" s="60"/>
+      <c r="AC15" s="60"/>
+      <c r="AD15" s="60"/>
     </row>
     <row r="16" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B16" s="55"/>
-      <c r="C16" s="55"/>
-      <c r="D16" s="55"/>
-      <c r="E16" s="55"/>
-      <c r="F16" s="55"/>
-      <c r="Z16" s="53"/>
-      <c r="AA16" s="53"/>
-      <c r="AB16" s="53"/>
-      <c r="AC16" s="53"/>
-      <c r="AD16" s="53"/>
+      <c r="B16" s="62"/>
+      <c r="C16" s="62"/>
+      <c r="D16" s="62"/>
+      <c r="E16" s="62"/>
+      <c r="F16" s="62"/>
+      <c r="Z16" s="60"/>
+      <c r="AA16" s="60"/>
+      <c r="AB16" s="60"/>
+      <c r="AC16" s="60"/>
+      <c r="AD16" s="60"/>
     </row>
     <row r="17" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B17" s="55"/>
-      <c r="C17" s="55"/>
-      <c r="D17" s="55"/>
-      <c r="E17" s="55"/>
-      <c r="F17" s="55"/>
-      <c r="Z17" s="53"/>
-      <c r="AA17" s="53"/>
-      <c r="AB17" s="53"/>
-      <c r="AC17" s="53"/>
-      <c r="AD17" s="53"/>
+      <c r="B17" s="62"/>
+      <c r="C17" s="62"/>
+      <c r="D17" s="62"/>
+      <c r="E17" s="62"/>
+      <c r="F17" s="62"/>
+      <c r="Z17" s="60"/>
+      <c r="AA17" s="60"/>
+      <c r="AB17" s="60"/>
+      <c r="AC17" s="60"/>
+      <c r="AD17" s="60"/>
     </row>
     <row r="18" spans="2:30" x14ac:dyDescent="0.35">
       <c r="B18" s="24"/>
@@ -8235,11 +8235,11 @@
       <c r="D18" s="24"/>
       <c r="E18" s="24"/>
       <c r="F18" s="24"/>
-      <c r="Z18" s="53"/>
-      <c r="AA18" s="53"/>
-      <c r="AB18" s="53"/>
-      <c r="AC18" s="53"/>
-      <c r="AD18" s="53"/>
+      <c r="Z18" s="60"/>
+      <c r="AA18" s="60"/>
+      <c r="AB18" s="60"/>
+      <c r="AC18" s="60"/>
+      <c r="AD18" s="60"/>
     </row>
     <row r="19" spans="2:30" x14ac:dyDescent="0.35">
       <c r="B19" s="24"/>
@@ -8247,263 +8247,263 @@
       <c r="D19" s="24"/>
       <c r="E19" s="24"/>
       <c r="F19" s="24"/>
-      <c r="Z19" s="53"/>
-      <c r="AA19" s="53"/>
-      <c r="AB19" s="53"/>
-      <c r="AC19" s="53"/>
-      <c r="AD19" s="53"/>
+      <c r="Z19" s="60"/>
+      <c r="AA19" s="60"/>
+      <c r="AB19" s="60"/>
+      <c r="AC19" s="60"/>
+      <c r="AD19" s="60"/>
     </row>
     <row r="20" spans="2:30" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="55" t="s">
+      <c r="B20" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="55"/>
-      <c r="D20" s="55"/>
-      <c r="E20" s="55"/>
-      <c r="F20" s="55"/>
-      <c r="Z20" s="53"/>
-      <c r="AA20" s="53"/>
-      <c r="AB20" s="53"/>
-      <c r="AC20" s="53"/>
-      <c r="AD20" s="53"/>
+      <c r="C20" s="62"/>
+      <c r="D20" s="62"/>
+      <c r="E20" s="62"/>
+      <c r="F20" s="62"/>
+      <c r="Z20" s="60"/>
+      <c r="AA20" s="60"/>
+      <c r="AB20" s="60"/>
+      <c r="AC20" s="60"/>
+      <c r="AD20" s="60"/>
     </row>
     <row r="21" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B21" s="55"/>
-      <c r="C21" s="55"/>
-      <c r="D21" s="55"/>
-      <c r="E21" s="55"/>
-      <c r="F21" s="55"/>
-      <c r="Z21" s="53"/>
-      <c r="AA21" s="53"/>
-      <c r="AB21" s="53"/>
-      <c r="AC21" s="53"/>
-      <c r="AD21" s="53"/>
+      <c r="B21" s="62"/>
+      <c r="C21" s="62"/>
+      <c r="D21" s="62"/>
+      <c r="E21" s="62"/>
+      <c r="F21" s="62"/>
+      <c r="Z21" s="60"/>
+      <c r="AA21" s="60"/>
+      <c r="AB21" s="60"/>
+      <c r="AC21" s="60"/>
+      <c r="AD21" s="60"/>
     </row>
     <row r="22" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B22" s="55"/>
-      <c r="C22" s="55"/>
-      <c r="D22" s="55"/>
-      <c r="E22" s="55"/>
-      <c r="F22" s="55"/>
-      <c r="Z22" s="53"/>
-      <c r="AA22" s="53"/>
-      <c r="AB22" s="53"/>
-      <c r="AC22" s="53"/>
-      <c r="AD22" s="53"/>
+      <c r="B22" s="62"/>
+      <c r="C22" s="62"/>
+      <c r="D22" s="62"/>
+      <c r="E22" s="62"/>
+      <c r="F22" s="62"/>
+      <c r="Z22" s="60"/>
+      <c r="AA22" s="60"/>
+      <c r="AB22" s="60"/>
+      <c r="AC22" s="60"/>
+      <c r="AD22" s="60"/>
     </row>
     <row r="23" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B23" s="55"/>
-      <c r="C23" s="55"/>
-      <c r="D23" s="55"/>
-      <c r="E23" s="55"/>
-      <c r="F23" s="55"/>
-      <c r="Z23" s="53"/>
-      <c r="AA23" s="53"/>
-      <c r="AB23" s="53"/>
-      <c r="AC23" s="53"/>
-      <c r="AD23" s="53"/>
+      <c r="B23" s="62"/>
+      <c r="C23" s="62"/>
+      <c r="D23" s="62"/>
+      <c r="E23" s="62"/>
+      <c r="F23" s="62"/>
+      <c r="Z23" s="60"/>
+      <c r="AA23" s="60"/>
+      <c r="AB23" s="60"/>
+      <c r="AC23" s="60"/>
+      <c r="AD23" s="60"/>
     </row>
     <row r="24" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B24" s="55"/>
-      <c r="C24" s="55"/>
-      <c r="D24" s="55"/>
-      <c r="E24" s="55"/>
-      <c r="F24" s="55"/>
-      <c r="Z24" s="53"/>
-      <c r="AA24" s="53"/>
-      <c r="AB24" s="53"/>
-      <c r="AC24" s="53"/>
-      <c r="AD24" s="53"/>
+      <c r="B24" s="62"/>
+      <c r="C24" s="62"/>
+      <c r="D24" s="62"/>
+      <c r="E24" s="62"/>
+      <c r="F24" s="62"/>
+      <c r="Z24" s="60"/>
+      <c r="AA24" s="60"/>
+      <c r="AB24" s="60"/>
+      <c r="AC24" s="60"/>
+      <c r="AD24" s="60"/>
     </row>
     <row r="25" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B25" s="55"/>
-      <c r="C25" s="55"/>
-      <c r="D25" s="55"/>
-      <c r="E25" s="55"/>
-      <c r="F25" s="55"/>
-      <c r="Z25" s="53"/>
-      <c r="AA25" s="53"/>
-      <c r="AB25" s="53"/>
-      <c r="AC25" s="53"/>
-      <c r="AD25" s="53"/>
+      <c r="B25" s="62"/>
+      <c r="C25" s="62"/>
+      <c r="D25" s="62"/>
+      <c r="E25" s="62"/>
+      <c r="F25" s="62"/>
+      <c r="Z25" s="60"/>
+      <c r="AA25" s="60"/>
+      <c r="AB25" s="60"/>
+      <c r="AC25" s="60"/>
+      <c r="AD25" s="60"/>
     </row>
     <row r="26" spans="2:30" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B26" s="55"/>
-      <c r="C26" s="55"/>
-      <c r="D26" s="55"/>
-      <c r="E26" s="55"/>
-      <c r="F26" s="55"/>
-      <c r="Z26" s="58" t="str">
+      <c r="B26" s="62"/>
+      <c r="C26" s="62"/>
+      <c r="D26" s="62"/>
+      <c r="E26" s="62"/>
+      <c r="F26" s="62"/>
+      <c r="Z26" s="65" t="str">
         <f>HYPERLINK("https://duet3d.dozuki.com/Wiki/Gcode#Section_M911_Configure_auto_save_on_loss_of_power","Read more: -&gt; M911 Gcode &lt;-")</f>
         <v>Read more: -&gt; M911 Gcode &lt;-</v>
       </c>
-      <c r="AA26" s="58"/>
-      <c r="AB26" s="58"/>
-      <c r="AC26" s="58"/>
-      <c r="AD26" s="58"/>
+      <c r="AA26" s="65"/>
+      <c r="AB26" s="65"/>
+      <c r="AC26" s="65"/>
+      <c r="AD26" s="65"/>
     </row>
     <row r="29" spans="2:30" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="54" t="s">
+      <c r="B29" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="C29" s="54"/>
-      <c r="D29" s="54"/>
-      <c r="E29" s="54"/>
-      <c r="F29" s="54"/>
-      <c r="Z29" s="60" t="s">
+      <c r="C29" s="61"/>
+      <c r="D29" s="61"/>
+      <c r="E29" s="61"/>
+      <c r="F29" s="61"/>
+      <c r="Z29" s="67" t="s">
         <v>45</v>
       </c>
-      <c r="AA29" s="60"/>
-      <c r="AB29" s="60"/>
-      <c r="AC29" s="60"/>
-      <c r="AD29" s="60"/>
+      <c r="AA29" s="67"/>
+      <c r="AB29" s="67"/>
+      <c r="AC29" s="67"/>
+      <c r="AD29" s="67"/>
     </row>
     <row r="30" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B30" s="54"/>
-      <c r="C30" s="54"/>
-      <c r="D30" s="54"/>
-      <c r="E30" s="54"/>
-      <c r="F30" s="54"/>
-      <c r="Z30" s="60"/>
-      <c r="AA30" s="60"/>
-      <c r="AB30" s="60"/>
-      <c r="AC30" s="60"/>
-      <c r="AD30" s="60"/>
+      <c r="B30" s="61"/>
+      <c r="C30" s="61"/>
+      <c r="D30" s="61"/>
+      <c r="E30" s="61"/>
+      <c r="F30" s="61"/>
+      <c r="Z30" s="67"/>
+      <c r="AA30" s="67"/>
+      <c r="AB30" s="67"/>
+      <c r="AC30" s="67"/>
+      <c r="AD30" s="67"/>
     </row>
     <row r="31" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B31" s="54"/>
-      <c r="C31" s="54"/>
-      <c r="D31" s="54"/>
-      <c r="E31" s="54"/>
-      <c r="F31" s="54"/>
-      <c r="Z31" s="60"/>
-      <c r="AA31" s="60"/>
-      <c r="AB31" s="60"/>
-      <c r="AC31" s="60"/>
-      <c r="AD31" s="60"/>
+      <c r="B31" s="61"/>
+      <c r="C31" s="61"/>
+      <c r="D31" s="61"/>
+      <c r="E31" s="61"/>
+      <c r="F31" s="61"/>
+      <c r="Z31" s="67"/>
+      <c r="AA31" s="67"/>
+      <c r="AB31" s="67"/>
+      <c r="AC31" s="67"/>
+      <c r="AD31" s="67"/>
     </row>
     <row r="32" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="Z32" s="60"/>
-      <c r="AA32" s="60"/>
-      <c r="AB32" s="60"/>
-      <c r="AC32" s="60"/>
-      <c r="AD32" s="60"/>
+      <c r="Z32" s="67"/>
+      <c r="AA32" s="67"/>
+      <c r="AB32" s="67"/>
+      <c r="AC32" s="67"/>
+      <c r="AD32" s="67"/>
     </row>
     <row r="33" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="Z33" s="60"/>
-      <c r="AA33" s="60"/>
-      <c r="AB33" s="60"/>
-      <c r="AC33" s="60"/>
-      <c r="AD33" s="60"/>
+      <c r="Z33" s="67"/>
+      <c r="AA33" s="67"/>
+      <c r="AB33" s="67"/>
+      <c r="AC33" s="67"/>
+      <c r="AD33" s="67"/>
     </row>
     <row r="34" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B34" s="53" t="s">
+      <c r="B34" s="60" t="s">
         <v>46</v>
       </c>
-      <c r="C34" s="53"/>
-      <c r="D34" s="53"/>
-      <c r="E34" s="53"/>
-      <c r="F34" s="53"/>
-      <c r="Z34" s="60"/>
-      <c r="AA34" s="60"/>
-      <c r="AB34" s="60"/>
-      <c r="AC34" s="60"/>
-      <c r="AD34" s="60"/>
+      <c r="C34" s="60"/>
+      <c r="D34" s="60"/>
+      <c r="E34" s="60"/>
+      <c r="F34" s="60"/>
+      <c r="Z34" s="67"/>
+      <c r="AA34" s="67"/>
+      <c r="AB34" s="67"/>
+      <c r="AC34" s="67"/>
+      <c r="AD34" s="67"/>
     </row>
     <row r="35" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B35" s="53"/>
-      <c r="C35" s="53"/>
-      <c r="D35" s="53"/>
-      <c r="E35" s="53"/>
-      <c r="F35" s="53"/>
-      <c r="Z35" s="60"/>
-      <c r="AA35" s="60"/>
-      <c r="AB35" s="60"/>
-      <c r="AC35" s="60"/>
-      <c r="AD35" s="60"/>
+      <c r="B35" s="60"/>
+      <c r="C35" s="60"/>
+      <c r="D35" s="60"/>
+      <c r="E35" s="60"/>
+      <c r="F35" s="60"/>
+      <c r="Z35" s="67"/>
+      <c r="AA35" s="67"/>
+      <c r="AB35" s="67"/>
+      <c r="AC35" s="67"/>
+      <c r="AD35" s="67"/>
     </row>
     <row r="36" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B36" s="53"/>
-      <c r="C36" s="53"/>
-      <c r="D36" s="53"/>
-      <c r="E36" s="53"/>
-      <c r="F36" s="53"/>
-      <c r="Z36" s="60"/>
-      <c r="AA36" s="60"/>
-      <c r="AB36" s="60"/>
-      <c r="AC36" s="60"/>
-      <c r="AD36" s="60"/>
+      <c r="B36" s="60"/>
+      <c r="C36" s="60"/>
+      <c r="D36" s="60"/>
+      <c r="E36" s="60"/>
+      <c r="F36" s="60"/>
+      <c r="Z36" s="67"/>
+      <c r="AA36" s="67"/>
+      <c r="AB36" s="67"/>
+      <c r="AC36" s="67"/>
+      <c r="AD36" s="67"/>
     </row>
     <row r="37" spans="2:30" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="53"/>
-      <c r="C37" s="53"/>
-      <c r="D37" s="53"/>
-      <c r="E37" s="53"/>
-      <c r="F37" s="53"/>
-      <c r="Z37" s="60"/>
-      <c r="AA37" s="60"/>
-      <c r="AB37" s="60"/>
-      <c r="AC37" s="60"/>
-      <c r="AD37" s="60"/>
+      <c r="B37" s="60"/>
+      <c r="C37" s="60"/>
+      <c r="D37" s="60"/>
+      <c r="E37" s="60"/>
+      <c r="F37" s="60"/>
+      <c r="Z37" s="67"/>
+      <c r="AA37" s="67"/>
+      <c r="AB37" s="67"/>
+      <c r="AC37" s="67"/>
+      <c r="AD37" s="67"/>
     </row>
     <row r="38" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="Z38" s="60"/>
-      <c r="AA38" s="60"/>
-      <c r="AB38" s="60"/>
-      <c r="AC38" s="60"/>
-      <c r="AD38" s="60"/>
+      <c r="Z38" s="67"/>
+      <c r="AA38" s="67"/>
+      <c r="AB38" s="67"/>
+      <c r="AC38" s="67"/>
+      <c r="AD38" s="67"/>
     </row>
     <row r="39" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="Z39" s="60"/>
-      <c r="AA39" s="60"/>
-      <c r="AB39" s="60"/>
-      <c r="AC39" s="60"/>
-      <c r="AD39" s="60"/>
+      <c r="Z39" s="67"/>
+      <c r="AA39" s="67"/>
+      <c r="AB39" s="67"/>
+      <c r="AC39" s="67"/>
+      <c r="AD39" s="67"/>
     </row>
     <row r="40" spans="2:30" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="53" t="s">
+      <c r="B40" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="C40" s="53"/>
-      <c r="D40" s="53"/>
-      <c r="E40" s="53"/>
-      <c r="F40" s="53"/>
-      <c r="Z40" s="60"/>
-      <c r="AA40" s="60"/>
-      <c r="AB40" s="60"/>
-      <c r="AC40" s="60"/>
-      <c r="AD40" s="60"/>
+      <c r="C40" s="60"/>
+      <c r="D40" s="60"/>
+      <c r="E40" s="60"/>
+      <c r="F40" s="60"/>
+      <c r="Z40" s="67"/>
+      <c r="AA40" s="67"/>
+      <c r="AB40" s="67"/>
+      <c r="AC40" s="67"/>
+      <c r="AD40" s="67"/>
     </row>
     <row r="41" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B41" s="53"/>
-      <c r="C41" s="53"/>
-      <c r="D41" s="53"/>
-      <c r="E41" s="53"/>
-      <c r="F41" s="53"/>
-      <c r="Z41" s="60"/>
-      <c r="AA41" s="60"/>
-      <c r="AB41" s="60"/>
-      <c r="AC41" s="60"/>
-      <c r="AD41" s="60"/>
+      <c r="B41" s="60"/>
+      <c r="C41" s="60"/>
+      <c r="D41" s="60"/>
+      <c r="E41" s="60"/>
+      <c r="F41" s="60"/>
+      <c r="Z41" s="67"/>
+      <c r="AA41" s="67"/>
+      <c r="AB41" s="67"/>
+      <c r="AC41" s="67"/>
+      <c r="AD41" s="67"/>
     </row>
     <row r="42" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B42" s="53"/>
-      <c r="C42" s="53"/>
-      <c r="D42" s="53"/>
-      <c r="E42" s="53"/>
-      <c r="F42" s="53"/>
-      <c r="Z42" s="60"/>
-      <c r="AA42" s="60"/>
-      <c r="AB42" s="60"/>
-      <c r="AC42" s="60"/>
-      <c r="AD42" s="60"/>
+      <c r="B42" s="60"/>
+      <c r="C42" s="60"/>
+      <c r="D42" s="60"/>
+      <c r="E42" s="60"/>
+      <c r="F42" s="60"/>
+      <c r="Z42" s="67"/>
+      <c r="AA42" s="67"/>
+      <c r="AB42" s="67"/>
+      <c r="AC42" s="67"/>
+      <c r="AD42" s="67"/>
     </row>
     <row r="43" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B43" s="53"/>
-      <c r="C43" s="53"/>
-      <c r="D43" s="53"/>
-      <c r="E43" s="53"/>
-      <c r="F43" s="53"/>
+      <c r="B43" s="60"/>
+      <c r="C43" s="60"/>
+      <c r="D43" s="60"/>
+      <c r="E43" s="60"/>
+      <c r="F43" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -8551,27 +8551,27 @@
   </cols>
   <sheetData>
     <row r="6" spans="26:30" x14ac:dyDescent="0.35">
-      <c r="Z6" s="61" t="s">
+      <c r="Z6" s="68" t="s">
         <v>57</v>
       </c>
-      <c r="AA6" s="61"/>
-      <c r="AB6" s="61"/>
-      <c r="AC6" s="61"/>
-      <c r="AD6" s="61"/>
+      <c r="AA6" s="68"/>
+      <c r="AB6" s="68"/>
+      <c r="AC6" s="68"/>
+      <c r="AD6" s="68"/>
     </row>
     <row r="7" spans="26:30" x14ac:dyDescent="0.35">
-      <c r="Z7" s="61"/>
-      <c r="AA7" s="61"/>
-      <c r="AB7" s="61"/>
-      <c r="AC7" s="61"/>
-      <c r="AD7" s="61"/>
+      <c r="Z7" s="68"/>
+      <c r="AA7" s="68"/>
+      <c r="AB7" s="68"/>
+      <c r="AC7" s="68"/>
+      <c r="AD7" s="68"/>
     </row>
     <row r="8" spans="26:30" x14ac:dyDescent="0.35">
-      <c r="Z8" s="61"/>
-      <c r="AA8" s="61"/>
-      <c r="AB8" s="61"/>
-      <c r="AC8" s="61"/>
-      <c r="AD8" s="61"/>
+      <c r="Z8" s="68"/>
+      <c r="AA8" s="68"/>
+      <c r="AB8" s="68"/>
+      <c r="AC8" s="68"/>
+      <c r="AD8" s="68"/>
     </row>
     <row r="21" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="22" spans="2:7" x14ac:dyDescent="0.35">
@@ -8613,65 +8613,65 @@
     <row r="27" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B27" s="23"/>
       <c r="C27" s="25"/>
-      <c r="E27" s="53" t="s">
+      <c r="E27" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="F27" s="53"/>
-      <c r="G27" s="53"/>
+      <c r="F27" s="60"/>
+      <c r="G27" s="60"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B28" s="23"/>
       <c r="C28" s="25"/>
-      <c r="E28" s="53"/>
-      <c r="F28" s="53"/>
-      <c r="G28" s="53"/>
+      <c r="E28" s="60"/>
+      <c r="F28" s="60"/>
+      <c r="G28" s="60"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B29" s="23"/>
       <c r="C29" s="25"/>
-      <c r="E29" s="53"/>
-      <c r="F29" s="53"/>
-      <c r="G29" s="53"/>
+      <c r="E29" s="60"/>
+      <c r="F29" s="60"/>
+      <c r="G29" s="60"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B30" s="23"/>
       <c r="C30" s="25"/>
-      <c r="E30" s="53"/>
-      <c r="F30" s="53"/>
-      <c r="G30" s="53"/>
+      <c r="E30" s="60"/>
+      <c r="F30" s="60"/>
+      <c r="G30" s="60"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B31" s="23"/>
       <c r="C31" s="25"/>
-      <c r="E31" s="53"/>
-      <c r="F31" s="53"/>
-      <c r="G31" s="53"/>
+      <c r="E31" s="60"/>
+      <c r="F31" s="60"/>
+      <c r="G31" s="60"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B32" s="23"/>
       <c r="C32" s="25"/>
-      <c r="E32" s="53"/>
-      <c r="F32" s="53"/>
-      <c r="G32" s="53"/>
+      <c r="E32" s="60"/>
+      <c r="F32" s="60"/>
+      <c r="G32" s="60"/>
     </row>
     <row r="33" spans="2:30" x14ac:dyDescent="0.35">
       <c r="B33" s="23"/>
       <c r="C33" s="25"/>
-      <c r="E33" s="53"/>
-      <c r="F33" s="53"/>
-      <c r="G33" s="53"/>
+      <c r="E33" s="60"/>
+      <c r="F33" s="60"/>
+      <c r="G33" s="60"/>
     </row>
     <row r="34" spans="2:30" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B34" s="36"/>
       <c r="C34" s="27"/>
-      <c r="E34" s="53"/>
-      <c r="F34" s="53"/>
-      <c r="G34" s="53"/>
+      <c r="E34" s="60"/>
+      <c r="F34" s="60"/>
+      <c r="G34" s="60"/>
     </row>
     <row r="35" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="E35" s="53"/>
-      <c r="F35" s="53"/>
-      <c r="G35" s="53"/>
+      <c r="E35" s="60"/>
+      <c r="F35" s="60"/>
+      <c r="G35" s="60"/>
     </row>
     <row r="38" spans="2:30" x14ac:dyDescent="0.35">
       <c r="Z38" s="37"/>

</xml_diff>